<commit_message>
added information on the RCDI
</commit_message>
<xml_diff>
--- a/PartList.xlsx
+++ b/PartList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Instruments\SAXS002\TechnicalDrawings\ElectricalSafetyInterlock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Instruments\SAXS002\TechnicalDrawings\ElectricSafetyInterlock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13357611-0F3E-4860-99FF-D6674662AE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98959BE9-6E04-40A5-BA65-2B93CF6C24C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4AE3A097-5E3F-41B8-94E0-517968FFF5E1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>amount</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Kopp</t>
   </si>
   <si>
-    <t>B16A</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -207,6 +204,12 @@
   </si>
   <si>
     <t>System Power in connector w/switch</t>
+  </si>
+  <si>
+    <t>ABB DS202C</t>
+  </si>
+  <si>
+    <t>KS 68 B16A LS-DI</t>
   </si>
 </sst>
 </file>
@@ -261,17 +264,17 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,7 +593,7 @@
   <dimension ref="A2:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,37 +607,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -654,7 +657,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -676,7 +679,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -698,7 +701,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -717,7 +720,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -739,7 +742,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>18</v>
       </c>
@@ -761,12 +764,12 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="4"/>
       <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
         <v>41</v>
-      </c>
-      <c r="C10" t="s">
-        <v>42</v>
       </c>
       <c r="D10">
         <v>8771110</v>
@@ -789,8 +792,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>33</v>
+      <c r="A12" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
@@ -813,7 +816,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>25</v>
       </c>
@@ -835,9 +838,9 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="4"/>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -857,7 +860,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>28</v>
       </c>
@@ -865,26 +868,32 @@
         <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
+        <v>56</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
+      <c r="G15">
+        <v>136.80000000000001</v>
+      </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>136.80000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F16">
         <v>100</v>
@@ -898,15 +907,15 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="4"/>
       <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" t="s">
         <v>47</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
       </c>
       <c r="F17">
         <v>6</v>
@@ -920,18 +929,18 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="4"/>
       <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
         <v>49</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>50</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>51</v>
-      </c>
-      <c r="E18" t="s">
-        <v>52</v>
       </c>
       <c r="F18">
         <v>2</v>
@@ -945,15 +954,15 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="4"/>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F19">
         <v>6</v>
@@ -973,17 +982,17 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
         <v>34</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>35</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>36</v>
-      </c>
-      <c r="D21" t="s">
-        <v>37</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -997,15 +1006,15 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="4"/>
       <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
         <v>38</v>
-      </c>
-      <c r="C22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" t="s">
-        <v>39</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1019,12 +1028,12 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="4"/>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23">
         <v>467406</v>
@@ -1041,18 +1050,18 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="A25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
       <c r="H25">
         <f>SUM(H4:H23)</f>
-        <v>674.89</v>
+        <v>811.69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>